<commit_message>
Final OMs for changes to age specificity
</commit_message>
<xml_diff>
--- a/baseCaseOM/WMU42_StonesSheep_baseCase.xlsx
+++ b/baseCaseOM/WMU42_StonesSheep_baseCase.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Stock" sheetId="1" state="visible" r:id="rId2"/>
@@ -1244,8 +1244,8 @@
   </sheetPr>
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1523,26 +1523,14 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>0.7</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1785,7 +1773,7 @@
   <dimension ref="A1:AQ28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+      <selection pane="topLeft" activeCell="C22" activeCellId="1" sqref="B14:C15 C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2423,7 +2411,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
+      <selection pane="topLeft" activeCell="F16" activeCellId="1" sqref="B14:C15 F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2756,8 +2744,8 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C33" activeCellId="1" sqref="B14:C15 C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2865,7 +2853,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="B14:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>